<commit_message>
Fixed citation graph with full text
</commit_message>
<xml_diff>
--- a/Dataset/Covid_SLR_Dataset.xlsx
+++ b/Dataset/Covid_SLR_Dataset.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ethan\Desktop\2023USRAResearch\FASS-SLR\FASS-SLR\Dataset\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{856D3FA5-D25E-4A5D-AED8-AC86408C67C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31597757-B82F-4F4B-AB68-5A198C10A11B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5323,6 +5323,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="yyyy/mm/dd;@"/>
+  </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -5476,7 +5479,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
   </cellXfs>

</xml_diff>